<commit_message>
Kinda works, config file needs changes before turning in. Make sure the animals kill each other properly.
</commit_message>
<xml_diff>
--- a/AnimalCounts1.xlsx
+++ b/AnimalCounts1.xlsx
@@ -12,9 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Turn</t>
+  </si>
+  <si>
+    <t>Hare</t>
+  </si>
+  <si>
+    <t>Fox</t>
   </si>
 </sst>
 </file>
@@ -83,6 +89,1030 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hare</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>AnimalCounts!$A$2:$A$82</c:f>
+              <c:numCache>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnimalCounts!$B$2:$B$82</c:f>
+              <c:numCache>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>37.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Fox</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>AnimalCounts!$A$2:$A$82</c:f>
+              <c:numCache>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnimalCounts!$C$2:$C$82</c:f>
+              <c:numCache>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:axId val="0"/>
         <c:axId val="1"/>
       </c:lineChart>
@@ -207,7 +1237,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -217,11 +1247,23 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>0.0</v>
       </c>
+      <c r="B2" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -230,6 +1272,12 @@
       <c r="B3" t="n">
         <v>2.0</v>
       </c>
+      <c r="C3" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -238,6 +1286,12 @@
       <c r="B4" t="n">
         <v>4.0</v>
       </c>
+      <c r="C4" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -246,6 +1300,12 @@
       <c r="B5" t="n">
         <v>6.0</v>
       </c>
+      <c r="C5" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -254,6 +1314,12 @@
       <c r="B6" t="n">
         <v>8.0</v>
       </c>
+      <c r="C6" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -262,13 +1328,25 @@
       <c r="B7" t="n">
         <v>10.0</v>
       </c>
+      <c r="C7" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>6.0</v>
       </c>
       <c r="B8" t="n">
-        <v>12.0</v>
+        <v>11.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="9">
@@ -276,7 +1354,13 @@
         <v>7.0</v>
       </c>
       <c r="B9" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="10">
@@ -284,7 +1368,13 @@
         <v>8.0</v>
       </c>
       <c r="B10" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="11">
@@ -292,7 +1382,13 @@
         <v>9.0</v>
       </c>
       <c r="B11" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="12">
@@ -300,7 +1396,13 @@
         <v>10.0</v>
       </c>
       <c r="B12" t="n">
-        <v>14.0</v>
+        <v>17.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="13">
@@ -308,7 +1410,13 @@
         <v>11.0</v>
       </c>
       <c r="B13" t="n">
-        <v>14.0</v>
+        <v>18.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="14">
@@ -316,7 +1424,13 @@
         <v>12.0</v>
       </c>
       <c r="B14" t="n">
-        <v>14.0</v>
+        <v>19.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="15">
@@ -324,7 +1438,13 @@
         <v>13.0</v>
       </c>
       <c r="B15" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="16">
@@ -332,7 +1452,13 @@
         <v>14.0</v>
       </c>
       <c r="B16" t="n">
-        <v>14.0</v>
+        <v>23.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="17">
@@ -340,7 +1466,13 @@
         <v>15.0</v>
       </c>
       <c r="B17" t="n">
-        <v>14.0</v>
+        <v>25.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="18">
@@ -348,7 +1480,13 @@
         <v>16.0</v>
       </c>
       <c r="B18" t="n">
-        <v>14.0</v>
+        <v>27.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="19">
@@ -356,7 +1494,13 @@
         <v>17.0</v>
       </c>
       <c r="B19" t="n">
-        <v>14.0</v>
+        <v>29.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="20">
@@ -364,7 +1508,13 @@
         <v>18.0</v>
       </c>
       <c r="B20" t="n">
-        <v>14.0</v>
+        <v>31.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="21">
@@ -372,7 +1522,13 @@
         <v>19.0</v>
       </c>
       <c r="B21" t="n">
-        <v>14.0</v>
+        <v>33.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="22">
@@ -380,7 +1536,13 @@
         <v>20.0</v>
       </c>
       <c r="B22" t="n">
-        <v>14.0</v>
+        <v>35.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="23">
@@ -388,7 +1550,13 @@
         <v>21.0</v>
       </c>
       <c r="B23" t="n">
-        <v>14.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="24">
@@ -396,7 +1564,13 @@
         <v>22.0</v>
       </c>
       <c r="B24" t="n">
-        <v>14.0</v>
+        <v>36.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="25">
@@ -404,7 +1578,13 @@
         <v>23.0</v>
       </c>
       <c r="B25" t="n">
-        <v>14.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="26">
@@ -412,7 +1592,13 @@
         <v>24.0</v>
       </c>
       <c r="B26" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="27">
@@ -420,7 +1606,13 @@
         <v>25.0</v>
       </c>
       <c r="B27" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="28">
@@ -428,7 +1620,13 @@
         <v>26.0</v>
       </c>
       <c r="B28" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="29">
@@ -436,7 +1634,13 @@
         <v>27.0</v>
       </c>
       <c r="B29" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="30">
@@ -444,7 +1648,13 @@
         <v>28.0</v>
       </c>
       <c r="B30" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="31">
@@ -452,7 +1662,13 @@
         <v>29.0</v>
       </c>
       <c r="B31" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="32">
@@ -460,7 +1676,13 @@
         <v>30.0</v>
       </c>
       <c r="B32" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="33">
@@ -468,7 +1690,13 @@
         <v>31.0</v>
       </c>
       <c r="B33" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="34">
@@ -476,7 +1704,13 @@
         <v>32.0</v>
       </c>
       <c r="B34" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="35">
@@ -484,7 +1718,13 @@
         <v>33.0</v>
       </c>
       <c r="B35" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="36">
@@ -492,7 +1732,13 @@
         <v>34.0</v>
       </c>
       <c r="B36" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="37">
@@ -500,7 +1746,13 @@
         <v>35.0</v>
       </c>
       <c r="B37" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="38">
@@ -508,7 +1760,13 @@
         <v>36.0</v>
       </c>
       <c r="B38" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="39">
@@ -516,7 +1774,13 @@
         <v>37.0</v>
       </c>
       <c r="B39" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="40">
@@ -524,7 +1788,13 @@
         <v>38.0</v>
       </c>
       <c r="B40" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="41">
@@ -532,7 +1802,13 @@
         <v>39.0</v>
       </c>
       <c r="B41" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="42">
@@ -540,7 +1816,13 @@
         <v>40.0</v>
       </c>
       <c r="B42" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="43">
@@ -548,7 +1830,13 @@
         <v>41.0</v>
       </c>
       <c r="B43" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="44">
@@ -556,7 +1844,13 @@
         <v>42.0</v>
       </c>
       <c r="B44" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="45">
@@ -564,7 +1858,13 @@
         <v>43.0</v>
       </c>
       <c r="B45" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="46">
@@ -572,7 +1872,13 @@
         <v>44.0</v>
       </c>
       <c r="B46" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="47">
@@ -580,7 +1886,13 @@
         <v>45.0</v>
       </c>
       <c r="B47" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="48">
@@ -588,7 +1900,13 @@
         <v>46.0</v>
       </c>
       <c r="B48" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="49">
@@ -596,7 +1914,13 @@
         <v>47.0</v>
       </c>
       <c r="B49" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="50">
@@ -604,7 +1928,13 @@
         <v>48.0</v>
       </c>
       <c r="B50" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="51">
@@ -612,7 +1942,13 @@
         <v>49.0</v>
       </c>
       <c r="B51" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="52">
@@ -620,7 +1956,13 @@
         <v>50.0</v>
       </c>
       <c r="B52" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="53">
@@ -628,7 +1970,13 @@
         <v>51.0</v>
       </c>
       <c r="B53" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="54">
@@ -636,7 +1984,13 @@
         <v>52.0</v>
       </c>
       <c r="B54" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="55">
@@ -644,7 +1998,13 @@
         <v>53.0</v>
       </c>
       <c r="B55" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="56">
@@ -652,7 +2012,13 @@
         <v>54.0</v>
       </c>
       <c r="B56" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="57">
@@ -660,7 +2026,13 @@
         <v>55.0</v>
       </c>
       <c r="B57" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="58">
@@ -668,7 +2040,13 @@
         <v>56.0</v>
       </c>
       <c r="B58" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="59">
@@ -676,7 +2054,13 @@
         <v>57.0</v>
       </c>
       <c r="B59" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="60">
@@ -684,7 +2068,13 @@
         <v>58.0</v>
       </c>
       <c r="B60" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="61">
@@ -692,7 +2082,13 @@
         <v>59.0</v>
       </c>
       <c r="B61" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="62">
@@ -700,7 +2096,13 @@
         <v>60.0</v>
       </c>
       <c r="B62" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="63">
@@ -708,7 +2110,13 @@
         <v>61.0</v>
       </c>
       <c r="B63" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="64">
@@ -716,7 +2124,13 @@
         <v>62.0</v>
       </c>
       <c r="B64" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="65">
@@ -724,7 +2138,13 @@
         <v>63.0</v>
       </c>
       <c r="B65" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="66">
@@ -732,7 +2152,13 @@
         <v>64.0</v>
       </c>
       <c r="B66" t="n">
-        <v>14.0</v>
+        <v>41.0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="67">
@@ -740,7 +2166,13 @@
         <v>65.0</v>
       </c>
       <c r="B67" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="68">
@@ -748,7 +2180,13 @@
         <v>66.0</v>
       </c>
       <c r="B68" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="69">
@@ -756,7 +2194,13 @@
         <v>67.0</v>
       </c>
       <c r="B69" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="70">
@@ -764,7 +2208,13 @@
         <v>68.0</v>
       </c>
       <c r="B70" t="n">
-        <v>14.0</v>
+        <v>40.0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="71">
@@ -772,7 +2222,13 @@
         <v>69.0</v>
       </c>
       <c r="B71" t="n">
-        <v>14.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="72">
@@ -780,7 +2236,13 @@
         <v>70.0</v>
       </c>
       <c r="B72" t="n">
-        <v>14.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="73">
@@ -788,7 +2250,13 @@
         <v>71.0</v>
       </c>
       <c r="B73" t="n">
-        <v>14.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="74">
@@ -796,7 +2264,13 @@
         <v>72.0</v>
       </c>
       <c r="B74" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="75">
@@ -804,7 +2278,13 @@
         <v>73.0</v>
       </c>
       <c r="B75" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="76">
@@ -812,7 +2292,13 @@
         <v>74.0</v>
       </c>
       <c r="B76" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="77">
@@ -820,7 +2306,13 @@
         <v>75.0</v>
       </c>
       <c r="B77" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="78">
@@ -828,7 +2320,13 @@
         <v>76.0</v>
       </c>
       <c r="B78" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="79">
@@ -836,7 +2334,13 @@
         <v>77.0</v>
       </c>
       <c r="B79" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="80">
@@ -844,7 +2348,13 @@
         <v>78.0</v>
       </c>
       <c r="B80" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="81">
@@ -852,7 +2362,13 @@
         <v>79.0</v>
       </c>
       <c r="B81" t="n">
-        <v>14.0</v>
+        <v>38.0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>50.0</v>
       </c>
     </row>
     <row r="82">
@@ -860,7 +2376,13 @@
         <v>80.0</v>
       </c>
       <c r="B82" t="n">
-        <v>14.0</v>
+        <v>37.0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>50.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>